<commit_message>
update publications and presentations
</commit_message>
<xml_diff>
--- a/presentations.xlsx
+++ b/presentations.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="150">
   <si>
     <t>title</t>
   </si>
@@ -435,6 +435,36 @@
   </si>
   <si>
     <t>Bayesian estimation of true prevalence from apparent prevalence in R: Introducing the "prevalence" package</t>
+  </si>
+  <si>
+    <t>6th CYSTINET Working Group Meeting</t>
+  </si>
+  <si>
+    <t>Ljubljana, Slovenia</t>
+  </si>
+  <si>
+    <t>Assessment of the computer-based Taenia solium educational program 'The Vicious Worm' on knowledge update in primary school children in Katete district in Eastern Zambia</t>
+  </si>
+  <si>
+    <t>Hobbs, E C; Mwape, K E; Zulu, G; Mambwe, M; Chembensofu, M; Phiri, I K; Masuku, M; Berkvens, D; Bottieau, E; Devleesschauwer, Brecht; Speybroeck, Niko; Colston, A; Willingham, A L; Dorny, Pierre; Gabriël, Sarah</t>
+  </si>
+  <si>
+    <t>Risk factor analysis in patients with neurocysticercosis associated epilepsy in northern Uganda</t>
+  </si>
+  <si>
+    <t>Dupont, Fabian; Devleesschauwer, Brecht; Kaducu, Joyce; Lauseker, M; Schmidt, Veronika; Ovuga, E; Winkler, Andrea</t>
+  </si>
+  <si>
+    <t>Ranking foodborne parasites in Europe using multicriteria decision analyses</t>
+  </si>
+  <si>
+    <t>Bouwknegt, Martijn; Graham, Heather; Devleesschauwer, Brecht; Robertson, Lucy; van der Giessen, Joke</t>
+  </si>
+  <si>
+    <t>Joint EURO-FBP and CYSTINET Meeting</t>
+  </si>
+  <si>
+    <t>27</t>
   </si>
 </sst>
 </file>
@@ -566,8 +596,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:L24" totalsRowShown="0" headerRowDxfId="15">
-  <autoFilter ref="A1:L24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:L27" totalsRowShown="0" headerRowDxfId="15">
+  <autoFilter ref="A1:L27"/>
   <sortState ref="A2:L24">
     <sortCondition ref="L1:L24"/>
   </sortState>
@@ -900,9 +930,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1825,6 +1855,120 @@
       </c>
       <c r="L24" s="7">
         <v>42585</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>142</v>
+      </c>
+      <c r="B25" t="s">
+        <v>143</v>
+      </c>
+      <c r="C25" t="s">
+        <v>140</v>
+      </c>
+      <c r="D25">
+        <v>2016</v>
+      </c>
+      <c r="E25">
+        <v>9</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L25" s="7">
+        <v>42640</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>144</v>
+      </c>
+      <c r="B26" t="s">
+        <v>145</v>
+      </c>
+      <c r="C26" t="s">
+        <v>140</v>
+      </c>
+      <c r="D26">
+        <v>2016</v>
+      </c>
+      <c r="E26">
+        <v>9</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L26" s="7">
+        <v>42640</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>146</v>
+      </c>
+      <c r="B27" t="s">
+        <v>147</v>
+      </c>
+      <c r="C27" t="s">
+        <v>148</v>
+      </c>
+      <c r="D27">
+        <v>2016</v>
+      </c>
+      <c r="E27">
+        <v>9</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L27" s="7">
+        <v>42641</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update students and presentations
</commit_message>
<xml_diff>
--- a/presentations.xlsx
+++ b/presentations.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="168" windowWidth="14808" windowHeight="7956"/>
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="oral" sheetId="1" r:id="rId1"/>
     <sheet name="poster" sheetId="5" r:id="rId2"/>
+    <sheet name="oral-all" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="175">
   <si>
     <t>title</t>
   </si>
@@ -495,6 +496,51 @@
   </si>
   <si>
     <t>Bari, Italy</t>
+  </si>
+  <si>
+    <t>Changes in health in Belgium 1990--2015: a benchmarking analysis based on the Global Burden of Disease 2015 study</t>
+  </si>
+  <si>
+    <t>Maertens de Noordhout, Charline; Devleesschauwer, Brecht; Speybroeck, Niko</t>
+  </si>
+  <si>
+    <t>GBD 20th Anniversary Event</t>
+  </si>
+  <si>
+    <t>Seattle, WA, USA</t>
+  </si>
+  <si>
+    <t>WAAVP 2017</t>
+  </si>
+  <si>
+    <t>Estimates of the global and regional burden of foodborne parasites as determined by the World Health Organization</t>
+  </si>
+  <si>
+    <t>Seminar diagnosis and surveillance of infectious diseases WIV-ISP</t>
+  </si>
+  <si>
+    <t>The disease burden of infectious diseases in Belgium</t>
+  </si>
+  <si>
+    <t>Kuala Lumpur, Malaysia</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>Joint FAO/WHO Expert Meeting on Shiga Toxin-producing Escherichia coli (STEC)</t>
+  </si>
+  <si>
+    <t>WHO/FERG Estimates of the Global and Regional Burden of STEC</t>
+  </si>
+  <si>
+    <t>UCL Doctoral Day</t>
+  </si>
+  <si>
+    <t>Estimating the true burden of infectious diseases: methodological considerations</t>
   </si>
 </sst>
 </file>
@@ -559,7 +605,33 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="24">
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -626,7 +698,55 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:L28" totalsRowShown="0" headerRowDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:L17" totalsRowShown="0" headerRowDxfId="23">
+  <autoFilter ref="A1:L17"/>
+  <sortState ref="A2:L17">
+    <sortCondition ref="L1:L17"/>
+  </sortState>
+  <tableColumns count="12">
+    <tableColumn id="1" name="title"/>
+    <tableColumn id="2" name="authors"/>
+    <tableColumn id="13" name="conference"/>
+    <tableColumn id="3" name="year"/>
+    <tableColumn id="11" name="month"/>
+    <tableColumn id="6" name="day" dataDxfId="22"/>
+    <tableColumn id="4" name="location" dataDxfId="21"/>
+    <tableColumn id="5" name="journal" dataDxfId="20"/>
+    <tableColumn id="7" name="vol" dataDxfId="19"/>
+    <tableColumn id="14" name="suppl" dataDxfId="18"/>
+    <tableColumn id="8" name="page" dataDxfId="17"/>
+    <tableColumn id="10" name="date" dataDxfId="16"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabel14" displayName="Tabel14" ref="A1:L9" totalsRowShown="0" headerRowDxfId="15">
+  <autoFilter ref="A1:L9"/>
+  <sortState ref="A2:L5">
+    <sortCondition ref="L1:L5"/>
+  </sortState>
+  <tableColumns count="12">
+    <tableColumn id="1" name="title"/>
+    <tableColumn id="2" name="authors"/>
+    <tableColumn id="13" name="conference"/>
+    <tableColumn id="3" name="year"/>
+    <tableColumn id="11" name="month"/>
+    <tableColumn id="6" name="day" dataDxfId="14"/>
+    <tableColumn id="4" name="location" dataDxfId="13"/>
+    <tableColumn id="5" name="journal" dataDxfId="12"/>
+    <tableColumn id="7" name="vol" dataDxfId="11"/>
+    <tableColumn id="14" name="suppl" dataDxfId="10"/>
+    <tableColumn id="8" name="page" dataDxfId="9"/>
+    <tableColumn id="9" name="date" dataDxfId="8"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabel15" displayName="Tabel15" ref="A1:L28" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="A1:L28"/>
   <sortState ref="A2:L28">
     <sortCondition ref="L1:L28"/>
@@ -644,30 +764,6 @@
     <tableColumn id="14" name="suppl" dataDxfId="2"/>
     <tableColumn id="8" name="page" dataDxfId="1"/>
     <tableColumn id="10" name="date" dataDxfId="0"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabel14" displayName="Tabel14" ref="A1:L8" totalsRowShown="0" headerRowDxfId="15">
-  <autoFilter ref="A1:L8"/>
-  <sortState ref="A2:L5">
-    <sortCondition ref="L1:L5"/>
-  </sortState>
-  <tableColumns count="12">
-    <tableColumn id="1" name="title"/>
-    <tableColumn id="2" name="authors"/>
-    <tableColumn id="13" name="conference"/>
-    <tableColumn id="3" name="year"/>
-    <tableColumn id="11" name="month"/>
-    <tableColumn id="6" name="day" dataDxfId="14"/>
-    <tableColumn id="4" name="location" dataDxfId="13"/>
-    <tableColumn id="5" name="journal" dataDxfId="12"/>
-    <tableColumn id="7" name="vol" dataDxfId="11"/>
-    <tableColumn id="14" name="suppl" dataDxfId="10"/>
-    <tableColumn id="8" name="page" dataDxfId="9"/>
-    <tableColumn id="9" name="date" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -960,9 +1056,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1013,179 +1111,179 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D2">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="E2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>3</v>
+        <v>53</v>
+      </c>
+      <c r="I2" s="2">
+        <v>60</v>
+      </c>
+      <c r="J2" s="2">
+        <v>2</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="L2" s="7">
-        <v>40776</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+        <v>41252</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
       <c r="D3">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="E3">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="I3" s="2">
-        <v>22</v>
-      </c>
-      <c r="J3" s="2">
-        <v>2</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>61</v>
+        <v>3</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="L3" s="7">
-        <v>41132</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+        <v>41461</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
         <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="D4">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="E4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="I4" s="2">
-        <v>60</v>
-      </c>
-      <c r="J4" s="2">
-        <v>2</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>56</v>
+        <v>3</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="L4" s="7">
-        <v>41252</v>
+        <v>41566</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="D5">
         <v>2013</v>
       </c>
       <c r="E5">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>69</v>
+        <v>13</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>3</v>
+        <v>57</v>
+      </c>
+      <c r="I5" s="2">
+        <v>23</v>
+      </c>
+      <c r="J5" s="2">
+        <v>1</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="L5" s="7">
-        <v>41461</v>
+        <v>41592</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>16</v>
+      <c r="A6" s="5" t="s">
+        <v>139</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="D6">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="E6">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>3</v>
@@ -1196,34 +1294,34 @@
       <c r="J6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K6" s="2">
-        <v>12</v>
+      <c r="K6" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="L6" s="7">
-        <v>41533</v>
+        <v>41894</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>74</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>77</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="D7">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="E7">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>3</v>
@@ -1238,182 +1336,182 @@
         <v>3</v>
       </c>
       <c r="L7" s="7">
-        <v>41566</v>
+        <v>41946</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>73</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>63</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>78</v>
       </c>
       <c r="D8">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="E8">
         <v>11</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>13</v>
+        <v>71</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="I8" s="2">
-        <v>23</v>
-      </c>
-      <c r="J8" s="2">
-        <v>1</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>58</v>
+        <v>3</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="L8" s="7">
-        <v>41592</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+        <v>41961</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>103</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>63</v>
       </c>
       <c r="C9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D9">
+        <v>2015</v>
+      </c>
+      <c r="E9">
+        <v>12</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L9" s="7">
+        <v>42016</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10">
+        <v>2015</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L10" s="7">
+        <v>42213</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11">
+        <v>2015</v>
+      </c>
+      <c r="E11">
         <v>10</v>
       </c>
-      <c r="D9">
-        <v>2013</v>
-      </c>
-      <c r="E9">
-        <v>11</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="I9" s="2">
-        <v>23</v>
-      </c>
-      <c r="J9" s="2">
-        <v>1</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="L9" s="7">
-        <v>41592</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10">
-        <v>2013</v>
-      </c>
-      <c r="E10">
-        <v>11</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="I10" s="2">
-        <v>23</v>
-      </c>
-      <c r="J10" s="2">
-        <v>1</v>
-      </c>
-      <c r="K10" s="2">
-        <v>131</v>
-      </c>
-      <c r="L10" s="7">
-        <v>41592</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11">
-        <v>2013</v>
-      </c>
-      <c r="E11">
-        <v>11</v>
-      </c>
       <c r="F11" s="1" t="s">
-        <v>13</v>
+        <v>101</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>15</v>
+        <v>102</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="I11" s="2">
-        <v>23</v>
-      </c>
-      <c r="J11" s="2">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>60</v>
+        <v>3</v>
       </c>
       <c r="L11" s="7">
-        <v>41592</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>139</v>
+        <v>42303</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>106</v>
       </c>
       <c r="B12" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C12" t="s">
-        <v>66</v>
+        <v>107</v>
       </c>
       <c r="D12">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="E12">
         <v>12</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>64</v>
+        <v>108</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>65</v>
+        <v>109</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>3</v>
@@ -1428,30 +1526,30 @@
         <v>3</v>
       </c>
       <c r="L12" s="7">
-        <v>41894</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+        <v>42353</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>74</v>
+        <v>120</v>
       </c>
       <c r="B13" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="C13" t="s">
-        <v>76</v>
+        <v>116</v>
       </c>
       <c r="D13">
-        <v>2014</v>
+        <v>2016</v>
       </c>
       <c r="E13">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>75</v>
+        <v>119</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>15</v>
+        <v>121</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>3</v>
@@ -1466,30 +1564,30 @@
         <v>3</v>
       </c>
       <c r="L13" s="7">
-        <v>41946</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+        <v>42585</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>174</v>
       </c>
       <c r="B14" t="s">
         <v>63</v>
       </c>
       <c r="C14" t="s">
-        <v>78</v>
+        <v>173</v>
       </c>
       <c r="D14">
-        <v>2014</v>
+        <v>2016</v>
       </c>
       <c r="E14">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>72</v>
+        <v>15</v>
       </c>
       <c r="H14" s="4" t="s">
         <v>3</v>
@@ -1504,30 +1602,30 @@
         <v>3</v>
       </c>
       <c r="L14" s="7">
-        <v>41961</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+        <v>42642</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>103</v>
+        <v>167</v>
       </c>
       <c r="B15" t="s">
         <v>63</v>
       </c>
       <c r="C15" t="s">
-        <v>104</v>
+        <v>166</v>
       </c>
       <c r="D15">
-        <v>2015</v>
+        <v>2017</v>
       </c>
       <c r="E15">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>72</v>
+        <v>15</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>3</v>
@@ -1542,501 +1640,83 @@
         <v>3</v>
       </c>
       <c r="L15" s="7">
-        <v>42016</v>
+        <v>42873</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="D16" s="8">
-        <v>2015</v>
-      </c>
-      <c r="E16" s="9">
-        <v>5</v>
+      <c r="A16" t="s">
+        <v>165</v>
+      </c>
+      <c r="B16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" t="s">
+        <v>164</v>
+      </c>
+      <c r="D16">
+        <v>2017</v>
+      </c>
+      <c r="E16">
+        <v>9</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>129</v>
+        <v>169</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>130</v>
+        <v>168</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="I16" s="2">
-        <v>2015</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>131</v>
+        <v>3</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="L16" s="7">
-        <v>42144</v>
+        <v>42984</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>84</v>
+        <v>172</v>
       </c>
       <c r="B17" t="s">
         <v>63</v>
       </c>
       <c r="C17" t="s">
-        <v>85</v>
+        <v>171</v>
       </c>
       <c r="D17">
-        <v>2015</v>
+        <v>2017</v>
       </c>
       <c r="E17">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>86</v>
+        <v>170</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>46</v>
+        <v>136</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I17" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K17" s="2" t="s">
+      <c r="I17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K17" s="1" t="s">
         <v>3</v>
       </c>
       <c r="L17" s="7">
-        <v>42213</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>87</v>
-      </c>
-      <c r="B18" t="s">
-        <v>88</v>
-      </c>
-      <c r="C18" t="s">
-        <v>91</v>
-      </c>
-      <c r="D18">
-        <v>2015</v>
-      </c>
-      <c r="E18">
-        <v>7</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="L18" s="7">
-        <v>42264</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>92</v>
-      </c>
-      <c r="B19" t="s">
-        <v>93</v>
-      </c>
-      <c r="C19" t="s">
-        <v>96</v>
-      </c>
-      <c r="D19">
-        <v>2015</v>
-      </c>
-      <c r="E19">
-        <v>9</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="I19" s="2">
-        <v>73</v>
-      </c>
-      <c r="J19" s="2">
-        <v>1</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="L19" s="7">
-        <v>42264</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>98</v>
-      </c>
-      <c r="B20" t="s">
-        <v>99</v>
-      </c>
-      <c r="C20" t="s">
-        <v>100</v>
-      </c>
-      <c r="D20">
-        <v>2015</v>
-      </c>
-      <c r="E20">
-        <v>10</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="L20" s="7">
-        <v>42303</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>106</v>
-      </c>
-      <c r="B21" t="s">
-        <v>63</v>
-      </c>
-      <c r="C21" t="s">
-        <v>107</v>
-      </c>
-      <c r="D21">
-        <v>2015</v>
-      </c>
-      <c r="E21">
-        <v>12</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="H21" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L21" s="7">
-        <v>42353</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>122</v>
-      </c>
-      <c r="B22" t="s">
-        <v>123</v>
-      </c>
-      <c r="C22" t="s">
-        <v>124</v>
-      </c>
-      <c r="D22">
-        <v>2016</v>
-      </c>
-      <c r="E22">
-        <v>3</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L22" s="7">
-        <v>42446</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>155</v>
-      </c>
-      <c r="B23" t="s">
-        <v>156</v>
-      </c>
-      <c r="C23" t="s">
-        <v>157</v>
-      </c>
-      <c r="D23">
-        <v>2016</v>
-      </c>
-      <c r="E23">
-        <v>6</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L23" s="7">
-        <v>42542</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>117</v>
-      </c>
-      <c r="B24" t="s">
-        <v>118</v>
-      </c>
-      <c r="C24" t="s">
-        <v>116</v>
-      </c>
-      <c r="D24">
-        <v>2016</v>
-      </c>
-      <c r="E24">
-        <v>8</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L24" s="7">
-        <v>42585</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>120</v>
-      </c>
-      <c r="B25" t="s">
-        <v>63</v>
-      </c>
-      <c r="C25" t="s">
-        <v>116</v>
-      </c>
-      <c r="D25">
-        <v>2016</v>
-      </c>
-      <c r="E25">
-        <v>8</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L25" s="7">
-        <v>42585</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>142</v>
-      </c>
-      <c r="B26" t="s">
-        <v>143</v>
-      </c>
-      <c r="C26" t="s">
-        <v>140</v>
-      </c>
-      <c r="D26">
-        <v>2016</v>
-      </c>
-      <c r="E26">
-        <v>9</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L26" s="7">
-        <v>42640</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>144</v>
-      </c>
-      <c r="B27" t="s">
-        <v>145</v>
-      </c>
-      <c r="C27" t="s">
-        <v>140</v>
-      </c>
-      <c r="D27">
-        <v>2016</v>
-      </c>
-      <c r="E27">
-        <v>9</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L27" s="7">
-        <v>42640</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>146</v>
-      </c>
-      <c r="B28" t="s">
-        <v>147</v>
-      </c>
-      <c r="C28" t="s">
-        <v>148</v>
-      </c>
-      <c r="D28">
-        <v>2016</v>
-      </c>
-      <c r="E28">
-        <v>9</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L28" s="7">
-        <v>42641</v>
+        <v>43003</v>
       </c>
     </row>
   </sheetData>
@@ -2050,7 +1730,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
@@ -2369,10 +2049,1140 @@
         <v>42687</v>
       </c>
     </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>160</v>
+      </c>
+      <c r="B9" t="s">
+        <v>161</v>
+      </c>
+      <c r="C9" t="s">
+        <v>162</v>
+      </c>
+      <c r="D9">
+        <v>2017</v>
+      </c>
+      <c r="E9">
+        <v>9</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="L9" s="7">
+        <v>43003</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L28"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="3" width="25.6640625" customWidth="1"/>
+    <col min="4" max="5" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="20.6640625" style="1" customWidth="1"/>
+    <col min="9" max="11" width="8.88671875" style="2"/>
+    <col min="12" max="12" width="15.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2">
+        <v>2011</v>
+      </c>
+      <c r="E2">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="7">
+        <v>40776</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3">
+        <v>2012</v>
+      </c>
+      <c r="E3">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="I3" s="2">
+        <v>22</v>
+      </c>
+      <c r="J3" s="2">
+        <v>2</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="L3" s="7">
+        <v>41132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4">
+        <v>2012</v>
+      </c>
+      <c r="E4">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I4" s="2">
+        <v>60</v>
+      </c>
+      <c r="J4" s="2">
+        <v>2</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="L4" s="7">
+        <v>41252</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5">
+        <v>2013</v>
+      </c>
+      <c r="E5">
+        <v>6</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L5" s="7">
+        <v>41461</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6">
+        <v>2013</v>
+      </c>
+      <c r="E6">
+        <v>9</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K6" s="2">
+        <v>12</v>
+      </c>
+      <c r="L6" s="7">
+        <v>41533</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7">
+        <v>2013</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L7" s="7">
+        <v>41566</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>2013</v>
+      </c>
+      <c r="E8">
+        <v>11</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="I8" s="2">
+        <v>23</v>
+      </c>
+      <c r="J8" s="2">
+        <v>1</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L8" s="7">
+        <v>41592</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>2013</v>
+      </c>
+      <c r="E9">
+        <v>11</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="I9" s="2">
+        <v>23</v>
+      </c>
+      <c r="J9" s="2">
+        <v>1</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="L9" s="7">
+        <v>41592</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <v>2013</v>
+      </c>
+      <c r="E10">
+        <v>11</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="I10" s="2">
+        <v>23</v>
+      </c>
+      <c r="J10" s="2">
+        <v>1</v>
+      </c>
+      <c r="K10" s="2">
+        <v>131</v>
+      </c>
+      <c r="L10" s="7">
+        <v>41592</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>2013</v>
+      </c>
+      <c r="E11">
+        <v>11</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="I11" s="2">
+        <v>23</v>
+      </c>
+      <c r="J11" s="2">
+        <v>1</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="L11" s="7">
+        <v>41592</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12">
+        <v>2014</v>
+      </c>
+      <c r="E12">
+        <v>12</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L12" s="7">
+        <v>41894</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13">
+        <v>2014</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L13" s="7">
+        <v>41946</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14">
+        <v>2014</v>
+      </c>
+      <c r="E14">
+        <v>11</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L14" s="7">
+        <v>41961</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>103</v>
+      </c>
+      <c r="B15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" t="s">
+        <v>104</v>
+      </c>
+      <c r="D15">
+        <v>2015</v>
+      </c>
+      <c r="E15">
+        <v>12</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L15" s="7">
+        <v>42016</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="D16" s="8">
+        <v>2015</v>
+      </c>
+      <c r="E16" s="9">
+        <v>5</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="I16" s="2">
+        <v>2015</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="L16" s="7">
+        <v>42144</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17">
+        <v>2015</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L17" s="7">
+        <v>42213</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18">
+        <v>2015</v>
+      </c>
+      <c r="E18">
+        <v>7</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L18" s="7">
+        <v>42264</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" t="s">
+        <v>93</v>
+      </c>
+      <c r="C19" t="s">
+        <v>96</v>
+      </c>
+      <c r="D19">
+        <v>2015</v>
+      </c>
+      <c r="E19">
+        <v>9</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="I19" s="2">
+        <v>73</v>
+      </c>
+      <c r="J19" s="2">
+        <v>1</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="L19" s="7">
+        <v>42264</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>98</v>
+      </c>
+      <c r="B20" t="s">
+        <v>99</v>
+      </c>
+      <c r="C20" t="s">
+        <v>100</v>
+      </c>
+      <c r="D20">
+        <v>2015</v>
+      </c>
+      <c r="E20">
+        <v>10</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L20" s="7">
+        <v>42303</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>106</v>
+      </c>
+      <c r="B21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" t="s">
+        <v>107</v>
+      </c>
+      <c r="D21">
+        <v>2015</v>
+      </c>
+      <c r="E21">
+        <v>12</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L21" s="7">
+        <v>42353</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>122</v>
+      </c>
+      <c r="B22" t="s">
+        <v>123</v>
+      </c>
+      <c r="C22" t="s">
+        <v>124</v>
+      </c>
+      <c r="D22">
+        <v>2016</v>
+      </c>
+      <c r="E22">
+        <v>3</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L22" s="7">
+        <v>42446</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>155</v>
+      </c>
+      <c r="B23" t="s">
+        <v>156</v>
+      </c>
+      <c r="C23" t="s">
+        <v>157</v>
+      </c>
+      <c r="D23">
+        <v>2016</v>
+      </c>
+      <c r="E23">
+        <v>6</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L23" s="7">
+        <v>42542</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>117</v>
+      </c>
+      <c r="B24" t="s">
+        <v>118</v>
+      </c>
+      <c r="C24" t="s">
+        <v>116</v>
+      </c>
+      <c r="D24">
+        <v>2016</v>
+      </c>
+      <c r="E24">
+        <v>8</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L24" s="7">
+        <v>42585</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>120</v>
+      </c>
+      <c r="B25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" t="s">
+        <v>116</v>
+      </c>
+      <c r="D25">
+        <v>2016</v>
+      </c>
+      <c r="E25">
+        <v>8</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L25" s="7">
+        <v>42585</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>142</v>
+      </c>
+      <c r="B26" t="s">
+        <v>143</v>
+      </c>
+      <c r="C26" t="s">
+        <v>140</v>
+      </c>
+      <c r="D26">
+        <v>2016</v>
+      </c>
+      <c r="E26">
+        <v>9</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L26" s="7">
+        <v>42640</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>144</v>
+      </c>
+      <c r="B27" t="s">
+        <v>145</v>
+      </c>
+      <c r="C27" t="s">
+        <v>140</v>
+      </c>
+      <c r="D27">
+        <v>2016</v>
+      </c>
+      <c r="E27">
+        <v>9</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L27" s="7">
+        <v>42640</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>146</v>
+      </c>
+      <c r="B28" t="s">
+        <v>147</v>
+      </c>
+      <c r="C28" t="s">
+        <v>148</v>
+      </c>
+      <c r="D28">
+        <v>2016</v>
+      </c>
+      <c r="E28">
+        <v>9</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L28" s="7">
+        <v>42641</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>